<commit_message>
commit email code changes
</commit_message>
<xml_diff>
--- a/src/test/java/TBR/Xlsdata_Files/Jobs.xlsx
+++ b/src/test/java/TBR/Xlsdata_Files/Jobs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10845" windowHeight="5115" tabRatio="885" firstSheet="9" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19275" windowHeight="9135" tabRatio="885" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="JobsClientAdd" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <definedName name="SectorClient">DataTextValidations!$B$3:$B$49</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:G15"/>
+  <oleSize ref="D1:M28"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="207">
   <si>
     <t>cname</t>
   </si>
@@ -653,6 +653,15 @@
   </si>
   <si>
     <t>deep</t>
+  </si>
+  <si>
+    <t>jack</t>
+  </si>
+  <si>
+    <t>CandidateAction</t>
+  </si>
+  <si>
+    <t>reject</t>
   </si>
 </sst>
 </file>
@@ -1277,7 +1286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1509,10 +1518,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BE2"/>
+  <dimension ref="A1:BF2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1522,18 +1531,18 @@
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
     <col min="4" max="9" width="17" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" customWidth="1"/>
-    <col min="11" max="14" width="17" customWidth="1"/>
-    <col min="15" max="15" width="15.7109375" customWidth="1"/>
-    <col min="16" max="16" width="18.140625" customWidth="1"/>
-    <col min="17" max="17" width="16.140625" customWidth="1"/>
-    <col min="18" max="18" width="20.28515625" customWidth="1"/>
-    <col min="19" max="19" width="19" customWidth="1"/>
-    <col min="20" max="20" width="18.5703125" customWidth="1"/>
-    <col min="21" max="21" width="21.28515625" customWidth="1"/>
-    <col min="22" max="22" width="11.7109375" customWidth="1"/>
+    <col min="11" max="15" width="17" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" customWidth="1"/>
+    <col min="17" max="17" width="18.140625" customWidth="1"/>
+    <col min="18" max="18" width="16.140625" customWidth="1"/>
+    <col min="19" max="19" width="20.28515625" customWidth="1"/>
+    <col min="20" max="20" width="19" customWidth="1"/>
+    <col min="21" max="21" width="18.5703125" customWidth="1"/>
+    <col min="22" max="22" width="21.28515625" customWidth="1"/>
+    <col min="23" max="23" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>67</v>
       </c>
@@ -1574,16 +1583,19 @@
         <v>151</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>190</v>
       </c>
@@ -1620,7 +1632,10 @@
         <v>160</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>192</v>
+        <v>206</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
19/01/2016 - extent reporting, select 31st code, updated test scripts
</commit_message>
<xml_diff>
--- a/src/test/java/TBR/Xlsdata_Files/Jobs.xlsx
+++ b/src/test/java/TBR/Xlsdata_Files/Jobs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11895" windowHeight="3795" tabRatio="885" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11895" windowHeight="3795" tabRatio="885" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="JobsClientAdd" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
     <definedName name="SectorClient">DataTextValidations!$B$3:$B$49</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:H10"/>
+  <oleSize ref="B1:G10"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="223">
   <si>
     <t>cname</t>
   </si>
@@ -707,6 +707,12 @@
   </si>
   <si>
     <t>jobAssignment</t>
+  </si>
+  <si>
+    <t>kiran</t>
+  </si>
+  <si>
+    <t>game</t>
   </si>
 </sst>
 </file>
@@ -1331,8 +1337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2125,7 +2131,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
@@ -2134,11 +2140,11 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="4" width="17.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="3" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -2148,17 +2154,20 @@
       <c r="C1" t="s">
         <v>195</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" t="s">
         <v>196</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>190</v>
       </c>
@@ -2168,7 +2177,10 @@
       <c r="C2" t="s">
         <v>212</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" t="s">
         <v>212</v>
       </c>
     </row>
@@ -2621,7 +2633,7 @@
         <v>205</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -3258,8 +3270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3364,7 +3376,7 @@
         <v>160</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>192</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -3390,7 +3402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>

</xml_diff>